<commit_message>
29 JLG loan scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3003-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-DISBURSE-FEE-%INTEREST-Regular-CASH-Newcreateloan.xlsx
+++ b/Mifos Automation Excels/Client/3003-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-DISBURSE-FEE-%INTEREST-Regular-CASH-Newcreateloan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="697" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="697" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -824,7 +824,7 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1617,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,7 +1742,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>